<commit_message>
multithreading + crm api connected
</commit_message>
<xml_diff>
--- a/airbnb/input_filter.xlsx
+++ b/airbnb/input_filter.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,386 +451,330 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45195</v>
+        <v>45206</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45196</v>
+        <v>45210</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45207</v>
+        <v>45215</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45211</v>
+        <v>45216</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45220</v>
+        <v>45221</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45222</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45227</v>
+        <v>45263</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45231</v>
+        <v>45267</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45234</v>
+        <v>45271</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45235</v>
+        <v>45273</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45238</v>
+        <v>45277</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45239</v>
+        <v>45279</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45243</v>
+        <v>45283</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45247</v>
+        <v>45285</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45255</v>
+        <v>45297</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45256</v>
+        <v>45301</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45264</v>
+        <v>45305</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45270</v>
+        <v>45306</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45271</v>
+        <v>45312</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45273</v>
+        <v>45313</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45276</v>
+        <v>45319</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>45278</v>
+        <v>45320</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45281</v>
+        <v>45320</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45284</v>
+        <v>45325</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45289</v>
+        <v>45330</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45290</v>
+        <v>45333</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45297</v>
+        <v>45334</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45299</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45302</v>
+        <v>45343</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45303</v>
+        <v>45347</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45308</v>
+        <v>45348</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45312</v>
+        <v>45350</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45319</v>
+        <v>45354</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45320</v>
+        <v>45360</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45334</v>
+        <v>45366</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>45340</v>
+        <v>45368</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45341</v>
+        <v>45369</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>45344</v>
+        <v>45375</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45349</v>
+        <v>45379</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>45354</v>
+        <v>45383</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45355</v>
+        <v>45387</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>45361</v>
+        <v>45392</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45362</v>
+        <v>45396</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>45364</v>
+        <v>45399</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45367</v>
+        <v>45403</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>45371</v>
+        <v>45404</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45376</v>
+        <v>45410</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>45382</v>
+        <v>45411</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45383</v>
+        <v>45417</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>45389</v>
+        <v>45418</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45394</v>
+        <v>45424</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>45398</v>
+        <v>45425</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45402</v>
+        <v>45431</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>45403</v>
+        <v>45432</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45404</v>
+        <v>45438</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>45410</v>
+        <v>45439</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45411</v>
+        <v>45445</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>45417</v>
+        <v>45446</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45418</v>
+        <v>45452</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>45424</v>
+        <v>45453</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45425</v>
+        <v>45459</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>45428</v>
+        <v>45460</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45440</v>
+        <v>45471</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>45445</v>
+        <v>45473</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45446</v>
+        <v>45474</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45452</v>
+        <v>45480</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45455</v>
+        <v>45481</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>45459</v>
+        <v>45485</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45460</v>
+        <v>45500</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>45466</v>
+        <v>45502</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45467</v>
+        <v>45516</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>45473</v>
+        <v>45520</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45474</v>
+        <v>45534</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>45480</v>
+        <v>45536</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45485</v>
+        <v>45537</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>45487</v>
+        <v>45543</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45488</v>
+        <v>45544</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>45494</v>
+        <v>45550</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45495</v>
+        <v>45551</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>45501</v>
+        <v>45557</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45502</v>
+        <v>45558</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>45508</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="2" t="n">
-        <v>45509</v>
-      </c>
-      <c r="B43" s="2" t="n">
-        <v>45515</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="2" t="n">
-        <v>45516</v>
-      </c>
-      <c r="B44" s="2" t="n">
-        <v>45522</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="2" t="n">
-        <v>45523</v>
-      </c>
-      <c r="B45" s="2" t="n">
-        <v>45529</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="2" t="n">
-        <v>45530</v>
-      </c>
-      <c r="B46" s="2" t="n">
-        <v>45536</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="2" t="n">
-        <v>45537</v>
-      </c>
-      <c r="B47" s="2" t="n">
-        <v>45543</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="2" t="n">
-        <v>45544</v>
-      </c>
-      <c r="B48" s="2" t="n">
-        <v>45550</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="2" t="n">
-        <v>45551</v>
-      </c>
-      <c r="B49" s="2" t="n">
-        <v>45554</v>
+        <v>45562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
other 3 sheets added
</commit_message>
<xml_diff>
--- a/airbnb/input_filter.xlsx
+++ b/airbnb/input_filter.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,330 +451,386 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45206</v>
+        <v>45207</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45210</v>
+        <v>45211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45215</v>
+        <v>45220</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45216</v>
+        <v>45222</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45221</v>
+        <v>45227</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45226</v>
+        <v>45231</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45263</v>
+        <v>45234</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45267</v>
+        <v>45235</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45271</v>
+        <v>45238</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45273</v>
+        <v>45239</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45277</v>
+        <v>45243</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45279</v>
+        <v>45247</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45283</v>
+        <v>45255</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45285</v>
+        <v>45256</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45297</v>
+        <v>45264</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45301</v>
+        <v>45270</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45305</v>
+        <v>45271</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45306</v>
+        <v>45273</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45312</v>
+        <v>45276</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45313</v>
+        <v>45278</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45319</v>
+        <v>45281</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>45320</v>
+        <v>45284</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45320</v>
+        <v>45289</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45325</v>
+        <v>45290</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45330</v>
+        <v>45297</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45333</v>
+        <v>45299</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45334</v>
+        <v>45302</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45338</v>
+        <v>45303</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45343</v>
+        <v>45308</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45347</v>
+        <v>45312</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45348</v>
+        <v>45319</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45350</v>
+        <v>45320</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45354</v>
+        <v>45334</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45360</v>
+        <v>45336</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45366</v>
+        <v>45339</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>45368</v>
+        <v>45344</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45369</v>
+        <v>45349</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>45375</v>
+        <v>45354</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45379</v>
+        <v>45355</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>45383</v>
+        <v>45361</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45387</v>
+        <v>45362</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>45392</v>
+        <v>45364</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45396</v>
+        <v>45367</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>45399</v>
+        <v>45371</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45403</v>
+        <v>45376</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>45404</v>
+        <v>45382</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45410</v>
+        <v>45383</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>45411</v>
+        <v>45389</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45417</v>
+        <v>45394</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>45418</v>
+        <v>45398</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45424</v>
+        <v>45402</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>45425</v>
+        <v>45403</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45431</v>
+        <v>45404</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>45432</v>
+        <v>45410</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45438</v>
+        <v>45411</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>45439</v>
+        <v>45417</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45445</v>
+        <v>45418</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>45446</v>
+        <v>45424</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45452</v>
+        <v>45425</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>45453</v>
+        <v>45428</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45459</v>
+        <v>45440</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>45460</v>
+        <v>45445</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45471</v>
+        <v>45446</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>45473</v>
+        <v>45452</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45474</v>
+        <v>45455</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45480</v>
+        <v>45459</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45481</v>
+        <v>45460</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>45485</v>
+        <v>45466</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45500</v>
+        <v>45467</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>45502</v>
+        <v>45473</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45516</v>
+        <v>45474</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>45520</v>
+        <v>45480</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45534</v>
+        <v>45485</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>45536</v>
+        <v>45487</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45537</v>
+        <v>45488</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>45543</v>
+        <v>45494</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45544</v>
+        <v>45495</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>45550</v>
+        <v>45501</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45551</v>
+        <v>45502</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>45557</v>
+        <v>45508</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
+        <v>45509</v>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>45515</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>45516</v>
+      </c>
+      <c r="B43" s="2" t="n">
+        <v>45522</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>45523</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>45529</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>45530</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>45537</v>
+      </c>
+      <c r="B46" s="2" t="n">
+        <v>45543</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>45544</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>45550</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>45551</v>
+      </c>
+      <c r="B48" s="2" t="n">
+        <v>45557</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
         <v>45558</v>
       </c>
-      <c r="B42" s="2" t="n">
-        <v>45562</v>
+      <c r="B49" s="2" t="n">
+        <v>45563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>